<commit_message>
A long overdue commit of many random changes.
</commit_message>
<xml_diff>
--- a/Na table enclosure/Na enclosure materials.xlsx
+++ b/Na table enclosure/Na enclosure materials.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="24030" windowHeight="7605"/>
+    <workbookView xWindow="-15" yWindow="7590" windowWidth="24030" windowHeight="7635"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
   <si>
     <t>Line #</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Length (inches)</t>
-  </si>
-  <si>
     <t>Additional machining operations</t>
   </si>
   <si>
@@ -97,6 +94,45 @@
   </si>
   <si>
     <t>7155 Cut to size 12.88 x 45 inches</t>
+  </si>
+  <si>
+    <t>Single tab end fastener</t>
+  </si>
+  <si>
+    <t>Double anchor fastener</t>
+  </si>
+  <si>
+    <t>Door hanger</t>
+  </si>
+  <si>
+    <t>Door glide</t>
+  </si>
+  <si>
+    <t>Inter-series hinge</t>
+  </si>
+  <si>
+    <t>Within-series hinge</t>
+  </si>
+  <si>
+    <t>Offset door handle</t>
+  </si>
+  <si>
+    <t>Interseries joining plate</t>
+  </si>
+  <si>
+    <t>10 series nut</t>
+  </si>
+  <si>
+    <t>15 series nut</t>
+  </si>
+  <si>
+    <t>170 feet</t>
+  </si>
+  <si>
+    <t>Rubber panel gasket</t>
+  </si>
+  <si>
+    <t>Cut to Length (inches)</t>
   </si>
 </sst>
 </file>
@@ -435,16 +471,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:I17"/>
+  <dimension ref="C3:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="26.7109375" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" customWidth="1"/>
+    <col min="7" max="8" width="22.42578125" customWidth="1"/>
     <col min="9" max="9" width="75.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -465,10 +501,10 @@
         <v>4</v>
       </c>
       <c r="H3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" t="s">
         <v>5</v>
-      </c>
-      <c r="I3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="3:9" x14ac:dyDescent="0.25">
@@ -482,16 +518,16 @@
         <v>2</v>
       </c>
       <c r="F4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" t="s">
         <v>7</v>
-      </c>
-      <c r="G4" t="s">
-        <v>8</v>
       </c>
       <c r="H4">
         <v>122.06</v>
       </c>
       <c r="I4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.25">
@@ -505,16 +541,16 @@
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H5">
         <v>60.19</v>
       </c>
       <c r="I5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="3:9" x14ac:dyDescent="0.25">
@@ -528,10 +564,10 @@
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H6">
         <v>52</v>
@@ -548,16 +584,16 @@
         <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H7">
         <v>50.5</v>
       </c>
       <c r="I7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.25">
@@ -571,16 +607,16 @@
         <v>4</v>
       </c>
       <c r="F8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H8">
-        <v>60.26</v>
+        <v>60.28</v>
       </c>
       <c r="I8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="3:9" x14ac:dyDescent="0.25">
@@ -594,10 +630,10 @@
         <v>8</v>
       </c>
       <c r="F10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H10">
         <v>57.88</v>
@@ -614,16 +650,16 @@
         <v>32</v>
       </c>
       <c r="F11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H11">
         <v>46.5</v>
       </c>
       <c r="I11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="3:9" x14ac:dyDescent="0.25">
@@ -637,16 +673,16 @@
         <v>16</v>
       </c>
       <c r="F12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H12">
         <v>13.5</v>
       </c>
       <c r="I12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.25">
@@ -660,16 +696,16 @@
         <v>16</v>
       </c>
       <c r="F13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H13">
         <v>12.38</v>
       </c>
       <c r="I13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="3:9" x14ac:dyDescent="0.25">
@@ -683,13 +719,13 @@
         <v>8</v>
       </c>
       <c r="F16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G16" t="s">
+        <v>23</v>
+      </c>
+      <c r="I16" t="s">
         <v>24</v>
-      </c>
-      <c r="I16" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.25">
@@ -703,13 +739,167 @@
         <v>8</v>
       </c>
       <c r="F17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" t="s">
         <v>23</v>
       </c>
-      <c r="G17" t="s">
+      <c r="I17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>12</v>
+      </c>
+      <c r="D21">
+        <v>3383</v>
+      </c>
+      <c r="E21">
+        <v>64</v>
+      </c>
+      <c r="G21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>13</v>
+      </c>
+      <c r="D22">
+        <v>3098</v>
+      </c>
+      <c r="E22">
         <v>24</v>
       </c>
-      <c r="I17" t="s">
-        <v>26</v>
+      <c r="G22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>14</v>
+      </c>
+      <c r="D23">
+        <v>2059</v>
+      </c>
+      <c r="E23">
+        <v>8</v>
+      </c>
+      <c r="G23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>15</v>
+      </c>
+      <c r="D24">
+        <v>2067</v>
+      </c>
+      <c r="E24">
+        <v>8</v>
+      </c>
+      <c r="G24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>16</v>
+      </c>
+      <c r="D25">
+        <v>2103</v>
+      </c>
+      <c r="E25">
+        <v>16</v>
+      </c>
+      <c r="G25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>17</v>
+      </c>
+      <c r="D26">
+        <v>2066</v>
+      </c>
+      <c r="E26">
+        <v>16</v>
+      </c>
+      <c r="G26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>18</v>
+      </c>
+      <c r="D27">
+        <v>2079</v>
+      </c>
+      <c r="E27">
+        <v>24</v>
+      </c>
+      <c r="G27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>19</v>
+      </c>
+      <c r="D28">
+        <v>4515</v>
+      </c>
+      <c r="E28">
+        <v>16</v>
+      </c>
+      <c r="G28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>20</v>
+      </c>
+      <c r="D29">
+        <v>3321</v>
+      </c>
+      <c r="E29">
+        <v>32</v>
+      </c>
+      <c r="G29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>21</v>
+      </c>
+      <c r="D30">
+        <v>3320</v>
+      </c>
+      <c r="E30">
+        <v>32</v>
+      </c>
+      <c r="G30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>22</v>
+      </c>
+      <c r="D31">
+        <v>2116</v>
+      </c>
+      <c r="E31" t="s">
+        <v>36</v>
+      </c>
+      <c r="G31" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>